<commit_message>
just some little modifs
</commit_message>
<xml_diff>
--- a/BL_Signal_Analysis/Bluetooth_Analysis.xlsx
+++ b/BL_Signal_Analysis/Bluetooth_Analysis.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julienchouvet/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julienchouvet/Documents/5_ISS/Context_Aware_IoT_System/Git/Team/Context-Aware-IoT-System/BL_Signal_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="460" windowWidth="28160" windowHeight="16820" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="460" windowWidth="28160" windowHeight="16820" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis in a classroom" sheetId="1" r:id="rId1"/>
@@ -239,14 +239,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -426,98 +419,98 @@
   </cellStyleXfs>
   <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -528,13 +521,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -864,7 +857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:P6"/>
     </sheetView>
   </sheetViews>
@@ -881,114 +874,114 @@
     </row>
     <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="6"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="15"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="9"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="18"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="9"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="18"/>
     </row>
     <row r="6" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="12"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="21"/>
     </row>
     <row r="8" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:16" ht="77" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="3"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="24"/>
     </row>
     <row r="10" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:16" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="23"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="26"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="O16" t="s">
@@ -997,74 +990,74 @@
     </row>
     <row r="41" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
-      <c r="P42" s="15"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="28"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="28"/>
+      <c r="J42" s="28"/>
+      <c r="K42" s="28"/>
+      <c r="L42" s="28"/>
+      <c r="M42" s="28"/>
+      <c r="N42" s="28"/>
+      <c r="O42" s="28"/>
+      <c r="P42" s="29"/>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B43" s="16"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="17"/>
-      <c r="J43" s="17"/>
-      <c r="K43" s="17"/>
-      <c r="L43" s="17"/>
-      <c r="M43" s="17"/>
-      <c r="N43" s="17"/>
-      <c r="O43" s="17"/>
-      <c r="P43" s="18"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="31"/>
+      <c r="H43" s="31"/>
+      <c r="I43" s="31"/>
+      <c r="J43" s="31"/>
+      <c r="K43" s="31"/>
+      <c r="L43" s="31"/>
+      <c r="M43" s="31"/>
+      <c r="N43" s="31"/>
+      <c r="O43" s="31"/>
+      <c r="P43" s="32"/>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B44" s="16"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
-      <c r="I44" s="17"/>
-      <c r="J44" s="17"/>
-      <c r="K44" s="17"/>
-      <c r="L44" s="17"/>
-      <c r="M44" s="17"/>
-      <c r="N44" s="17"/>
-      <c r="O44" s="17"/>
-      <c r="P44" s="18"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="31"/>
+      <c r="H44" s="31"/>
+      <c r="I44" s="31"/>
+      <c r="J44" s="31"/>
+      <c r="K44" s="31"/>
+      <c r="L44" s="31"/>
+      <c r="M44" s="31"/>
+      <c r="N44" s="31"/>
+      <c r="O44" s="31"/>
+      <c r="P44" s="32"/>
     </row>
     <row r="45" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="19"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
-      <c r="K45" s="20"/>
-      <c r="L45" s="20"/>
-      <c r="M45" s="20"/>
-      <c r="N45" s="20"/>
-      <c r="O45" s="20"/>
-      <c r="P45" s="21"/>
+      <c r="B45" s="33"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="34"/>
+      <c r="G45" s="34"/>
+      <c r="H45" s="34"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
+      <c r="K45" s="34"/>
+      <c r="L45" s="34"/>
+      <c r="M45" s="34"/>
+      <c r="N45" s="34"/>
+      <c r="O45" s="34"/>
+      <c r="P45" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1083,7 +1076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -1126,202 +1119,202 @@
       <c r="N4" s="38"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B5" s="24"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="26"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="26"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="3"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B6" s="24"/>
-      <c r="C6" s="27" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="8">
         <v>-75</v>
       </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="26"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="27" t="s">
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="31">
+      <c r="L6" s="8">
         <v>-83</v>
       </c>
-      <c r="M6" s="25"/>
-      <c r="N6" s="26"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="3"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B7" s="24"/>
-      <c r="C7" s="27" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="8">
         <v>-69</v>
       </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="26"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="27" t="s">
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="31">
+      <c r="L7" s="8">
         <v>-81</v>
       </c>
-      <c r="M7" s="25"/>
-      <c r="N7" s="26"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="3"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B8" s="24"/>
-      <c r="C8" s="27" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="8">
         <v>-74</v>
       </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="26"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="27" t="s">
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L8" s="31">
+      <c r="L8" s="8">
         <v>-79</v>
       </c>
-      <c r="M8" s="25"/>
-      <c r="N8" s="26"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="3"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B9" s="24"/>
-      <c r="C9" s="27" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="8">
         <v>-77</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="26"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="27" t="s">
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L9" s="32">
+      <c r="L9" s="9">
         <v>-80</v>
       </c>
-      <c r="M9" s="25"/>
-      <c r="N9" s="26"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="3"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B10" s="24"/>
-      <c r="C10" s="27" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="8">
         <v>-71</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="26"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="27" t="s">
+      <c r="E10" s="2"/>
+      <c r="F10" s="3"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L10" s="32">
+      <c r="L10" s="9">
         <v>-80</v>
       </c>
-      <c r="M10" s="25"/>
-      <c r="N10" s="26"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="3"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B11" s="24"/>
-      <c r="C11" s="27" t="s">
+      <c r="B11" s="1"/>
+      <c r="C11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="8">
         <v>-69</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="26"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="27" t="s">
+      <c r="E11" s="2"/>
+      <c r="F11" s="3"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L11" s="32">
+      <c r="L11" s="9">
         <v>-84</v>
       </c>
-      <c r="M11" s="25"/>
-      <c r="N11" s="26"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="3"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B12" s="24"/>
-      <c r="C12" s="27" t="s">
+      <c r="B12" s="1"/>
+      <c r="C12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="8">
         <v>-61</v>
       </c>
-      <c r="E12" s="25"/>
-      <c r="F12" s="26"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="27" t="s">
+      <c r="E12" s="2"/>
+      <c r="F12" s="3"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L12" s="32">
+      <c r="L12" s="9">
         <v>-86</v>
       </c>
-      <c r="M12" s="25"/>
-      <c r="N12" s="26"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="3"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B13" s="24"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="26"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="26"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="3"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="3"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B14" s="24"/>
-      <c r="C14" s="33" t="s">
+      <c r="B14" s="1"/>
+      <c r="C14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14" s="11">
         <f>AVERAGE(D6:D12)</f>
         <v>-70.857142857142861</v>
       </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="26"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="33" t="s">
+      <c r="E14" s="2"/>
+      <c r="F14" s="3"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L14" s="35">
+      <c r="L14" s="12">
         <f>AVERAGE(L6:L12)</f>
         <v>-81.857142857142861</v>
       </c>
-      <c r="M14" s="25"/>
-      <c r="N14" s="26"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="3"/>
     </row>
     <row r="15" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="28"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="30"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="30"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="7"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="7"/>
     </row>
     <row r="16" spans="2:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="2:15" ht="64" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>